<commit_message>
Changed authorizationType. authorizationCode data type from II to CD
</commit_message>
<xml_diff>
--- a/ServiceInteractions/riv/ehr/patientsummary/branches/TD_PATIENTSUMMARY_2/docs/CDA meddelandestruktur Vårddokument v1 10.xlsx
+++ b/ServiceInteractions/riv/ehr/patientsummary/branches/TD_PATIENTSUMMARY_2/docs/CDA meddelandestruktur Vårddokument v1 10.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22810"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="1815" windowWidth="11385" windowHeight="5610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27780" windowHeight="14860"/>
   </bookViews>
   <sheets>
     <sheet name="SendReferralAnswer CDA" sheetId="10" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -686,7 +691,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -733,6 +738,18 @@
       <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -784,17 +801,35 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -992,8 +1027,29 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="19">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1293,40 +1349,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Blad2">
+  <sheetPr codeName="Blad2" enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:AQ166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB78" sqref="AB78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
-    <col min="2" max="5" width="2.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
+    <col min="2" max="5" width="2.5" style="1" customWidth="1"/>
     <col min="6" max="8" width="3" style="1" customWidth="1"/>
-    <col min="9" max="12" width="3.42578125" style="1" customWidth="1"/>
-    <col min="13" max="17" width="3.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="5.5703125" style="1" customWidth="1"/>
+    <col min="9" max="12" width="3.5" style="1" customWidth="1"/>
+    <col min="13" max="17" width="3.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="5.5" style="1" customWidth="1"/>
     <col min="19" max="19" width="9" style="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="64.85546875" style="11" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" style="43" customWidth="1"/>
+    <col min="20" max="20" width="6.5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="64.83203125" style="11" customWidth="1"/>
+    <col min="22" max="22" width="7.5" style="43" customWidth="1"/>
     <col min="23" max="23" width="7" style="43" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1"/>
-    <col min="25" max="25" width="12.28515625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="8.7109375" style="51" customWidth="1"/>
-    <col min="28" max="28" width="10.5703125" style="51" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.5703125" style="51" customWidth="1"/>
-    <col min="30" max="30" width="64.28515625" style="72" customWidth="1"/>
-    <col min="31" max="16384" width="8.85546875" style="1"/>
+    <col min="24" max="24" width="8.83203125" style="1"/>
+    <col min="25" max="25" width="12.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5" style="1" customWidth="1"/>
+    <col min="27" max="27" width="8.6640625" style="51" customWidth="1"/>
+    <col min="28" max="28" width="10.5" style="51" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.5" style="51" customWidth="1"/>
+    <col min="30" max="30" width="64.33203125" style="72" customWidth="1"/>
+    <col min="31" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="2" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" s="2" customFormat="1" ht="2.25" customHeight="1">
       <c r="A1" s="40"/>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
@@ -1364,7 +1420,7 @@
       <c r="AI1" s="42"/>
       <c r="AQ1" s="10"/>
     </row>
-    <row r="2" spans="1:43" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" ht="6.75" customHeight="1">
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -1409,7 +1465,7 @@
       <c r="AP2" s="2"/>
       <c r="AQ2" s="2"/>
     </row>
-    <row r="3" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43" ht="27" customHeight="1">
       <c r="A3" s="74" t="s">
         <v>50</v>
       </c>
@@ -1450,7 +1506,7 @@
       <c r="AH3" s="42"/>
       <c r="AI3" s="43"/>
     </row>
-    <row r="4" spans="1:43" s="2" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:43" s="2" customFormat="1" ht="1.5" customHeight="1">
       <c r="A4" s="35"/>
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
@@ -1487,7 +1543,7 @@
       <c r="AH4" s="44"/>
       <c r="AI4" s="42"/>
     </row>
-    <row r="5" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:43" ht="30" customHeight="1">
       <c r="A5" s="33" t="s">
         <v>0</v>
       </c>
@@ -1532,7 +1588,7 @@
       <c r="AF5" s="45"/>
       <c r="AG5" s="45"/>
     </row>
-    <row r="6" spans="1:43" s="2" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:43" s="2" customFormat="1" ht="1.5" customHeight="1">
       <c r="A6" s="27"/>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
@@ -1567,7 +1623,7 @@
       <c r="AF6" s="26"/>
       <c r="AG6" s="26"/>
     </row>
-    <row r="7" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:43" ht="12.75" customHeight="1">
       <c r="A7" s="21" t="s">
         <v>150</v>
       </c>
@@ -1594,7 +1650,7 @@
       <c r="V7" s="55"/>
       <c r="W7" s="55"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="21" t="s">
         <v>53</v>
       </c>
@@ -1627,7 +1683,7 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="53"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" s="2" customFormat="1">
       <c r="A9" s="21" t="s">
         <v>150</v>
       </c>
@@ -1659,7 +1715,7 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="53"/>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1688,7 +1744,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" s="2" customFormat="1">
       <c r="A11"/>
       <c r="B11" t="s">
         <v>8</v>
@@ -1722,7 +1778,7 @@
       <c r="AC11" s="3"/>
       <c r="AD11" s="53"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" s="2" customFormat="1">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12" t="s">
@@ -1760,7 +1816,7 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="53"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13" t="s">
@@ -1792,7 +1848,7 @@
       <c r="V13" s="55"/>
       <c r="W13" s="55"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="24">
       <c r="A14"/>
       <c r="B14" t="s">
         <v>9</v>
@@ -1836,7 +1892,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" s="2" customFormat="1">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15" t="s">
@@ -1873,7 +1929,7 @@
       <c r="AC15" s="3"/>
       <c r="AD15" s="53"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="13.5" customHeight="1">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16" t="s">
@@ -1911,7 +1967,7 @@
       <c r="AC16" s="3"/>
       <c r="AD16" s="53"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30">
       <c r="A17"/>
       <c r="B17" t="s">
         <v>10</v>
@@ -1940,7 +1996,7 @@
       <c r="V17" s="18"/>
       <c r="W17" s="18"/>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18" t="s">
@@ -1973,7 +2029,7 @@
       <c r="V18" s="42"/>
       <c r="W18" s="42"/>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19" t="s">
@@ -2006,7 +2062,7 @@
       <c r="V19" s="18"/>
       <c r="W19" s="18"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30">
       <c r="A20"/>
       <c r="B20" t="s">
         <v>34</v>
@@ -2051,7 +2107,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" s="2" customFormat="1">
       <c r="A21"/>
       <c r="B21" t="s">
         <v>27</v>
@@ -2086,7 +2142,7 @@
       <c r="AC21" s="3"/>
       <c r="AD21" s="53"/>
     </row>
-    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" s="2" customFormat="1">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
@@ -2133,7 +2189,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" s="2" customFormat="1">
       <c r="A23" s="4"/>
       <c r="B23" s="6" t="s">
         <v>36</v>
@@ -2165,7 +2221,7 @@
       <c r="AC23" s="3"/>
       <c r="AD23" s="53"/>
     </row>
-    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" s="2" customFormat="1">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="6" t="s">
@@ -2203,7 +2259,7 @@
       <c r="AC24" s="3"/>
       <c r="AD24" s="53"/>
     </row>
-    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" s="2" customFormat="1">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="6" t="s">
@@ -2239,7 +2295,7 @@
       <c r="AC25" s="3"/>
       <c r="AD25" s="53"/>
     </row>
-    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" s="2" customFormat="1">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
         <v>11</v>
@@ -2274,7 +2330,7 @@
       <c r="AC26" s="3"/>
       <c r="AD26" s="53"/>
     </row>
-    <row r="27" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" s="2" customFormat="1">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="6" t="s">
@@ -2306,7 +2362,7 @@
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
     </row>
-    <row r="28" spans="1:30" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" s="2" customFormat="1" ht="36">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="6"/>
@@ -2348,7 +2404,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" s="2" customFormat="1">
       <c r="A29" s="4"/>
       <c r="B29" s="6"/>
       <c r="C29" s="4"/>
@@ -2387,7 +2443,7 @@
       <c r="AC29" s="3"/>
       <c r="AD29" s="53"/>
     </row>
-    <row r="30" spans="1:30" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" s="2" customFormat="1" ht="36">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="6"/>
@@ -2424,7 +2480,7 @@
       <c r="AC30" s="3"/>
       <c r="AD30" s="53"/>
     </row>
-    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" s="2" customFormat="1">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
         <v>13</v>
@@ -2466,7 +2522,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" s="2" customFormat="1">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="6" t="s">
@@ -2501,7 +2557,7 @@
       <c r="AC32" s="3"/>
       <c r="AD32" s="53"/>
     </row>
-    <row r="33" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31" s="2" customFormat="1">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2547,7 +2603,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:31" s="2" customFormat="1">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
@@ -2581,7 +2637,7 @@
       <c r="AD34" s="53"/>
       <c r="AE34" s="39"/>
     </row>
-    <row r="35" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2616,7 +2672,7 @@
       <c r="AC35" s="3"/>
       <c r="AD35" s="53"/>
     </row>
-    <row r="36" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2662,7 +2718,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2700,7 +2756,7 @@
       <c r="AC37" s="3"/>
       <c r="AD37" s="53"/>
     </row>
-    <row r="38" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2745,7 +2801,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2782,7 +2838,7 @@
       <c r="AC39" s="3"/>
       <c r="AD39" s="53"/>
     </row>
-    <row r="40" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2819,7 +2875,7 @@
       <c r="AC40" s="3"/>
       <c r="AD40" s="53"/>
     </row>
-    <row r="41" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2856,7 +2912,7 @@
       <c r="AC41" s="3"/>
       <c r="AD41" s="53"/>
     </row>
-    <row r="42" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2889,7 +2945,7 @@
       <c r="AC42" s="3"/>
       <c r="AD42" s="53"/>
     </row>
-    <row r="43" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2935,7 +2991,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
@@ -2967,7 +3023,7 @@
       <c r="AC44" s="3"/>
       <c r="AD44" s="53"/>
     </row>
-    <row r="45" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -3011,7 +3067,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="46" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -3048,7 +3104,7 @@
       <c r="AC46" s="3"/>
       <c r="AD46" s="53"/>
     </row>
-    <row r="47" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -3085,7 +3141,7 @@
       <c r="AC47" s="3"/>
       <c r="AD47" s="53"/>
     </row>
-    <row r="48" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -3132,7 +3188,7 @@
       </c>
       <c r="AE48" s="3"/>
     </row>
-    <row r="49" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -3178,7 +3234,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="50" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -3225,7 +3281,7 @@
       </c>
       <c r="AE50" s="3"/>
     </row>
-    <row r="51" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -3260,7 +3316,7 @@
       <c r="AC51" s="3"/>
       <c r="AD51" s="53"/>
     </row>
-    <row r="52" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -3293,7 +3349,7 @@
       <c r="AC52" s="3"/>
       <c r="AD52" s="53"/>
     </row>
-    <row r="53" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -3327,7 +3383,7 @@
       <c r="AC53" s="3"/>
       <c r="AD53" s="53"/>
     </row>
-    <row r="54" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -3372,7 +3428,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -3408,7 +3464,7 @@
       <c r="AC55" s="3"/>
       <c r="AD55" s="53"/>
     </row>
-    <row r="56" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:33" s="2" customFormat="1">
       <c r="A56" s="4"/>
       <c r="B56" s="4" t="s">
         <v>17</v>
@@ -3450,7 +3506,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:33" s="2" customFormat="1">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4" t="s">
@@ -3483,7 +3539,7 @@
       <c r="AC57" s="3"/>
       <c r="AD57" s="53"/>
     </row>
-    <row r="58" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:33" s="2" customFormat="1">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -3516,7 +3572,7 @@
       <c r="AC58" s="3"/>
       <c r="AD58" s="53"/>
     </row>
-    <row r="59" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:33" s="2" customFormat="1">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -3551,7 +3607,7 @@
       <c r="AC59" s="3"/>
       <c r="AD59" s="53"/>
     </row>
-    <row r="60" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:33" s="2" customFormat="1">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -3600,7 +3656,7 @@
       <c r="AF60" s="38"/>
       <c r="AG60" s="38"/>
     </row>
-    <row r="61" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:33" s="2" customFormat="1">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -3638,7 +3694,7 @@
       <c r="AC61" s="3"/>
       <c r="AD61" s="53"/>
     </row>
-    <row r="62" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:33" s="2" customFormat="1">
       <c r="A62" s="4"/>
       <c r="B62" s="4" t="s">
         <v>20</v>
@@ -3680,7 +3736,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:33" s="2" customFormat="1">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="6" t="s">
@@ -3713,7 +3769,7 @@
       <c r="AC63" s="3"/>
       <c r="AD63" s="53"/>
     </row>
-    <row r="64" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:33" s="2" customFormat="1" ht="24">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3761,7 +3817,7 @@
         <v>Tidpunkt för signering, format YYYYMMDDHHMMSS. RIV: Vård- och omsorgsdokument.signeringstidpunkt</v>
       </c>
     </row>
-    <row r="65" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:30" s="2" customFormat="1">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="6" t="s">
@@ -3794,7 +3850,7 @@
       <c r="AC65" s="3"/>
       <c r="AD65" s="53"/>
     </row>
-    <row r="66" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:30" s="2" customFormat="1">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -3830,7 +3886,7 @@
       <c r="AC66" s="3"/>
       <c r="AD66" s="3"/>
     </row>
-    <row r="67" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:30" s="2" customFormat="1">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4" t="s">
@@ -3870,7 +3926,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="68" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:30" s="2" customFormat="1">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -3905,7 +3961,7 @@
       <c r="AC68" s="3"/>
       <c r="AD68" s="3"/>
     </row>
-    <row r="69" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:30" s="2" customFormat="1">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -3951,7 +4007,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="70" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:30" s="2" customFormat="1">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -3989,7 +4045,7 @@
       <c r="AC70" s="3"/>
       <c r="AD70" s="53"/>
     </row>
-    <row r="71" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:30" s="2" customFormat="1">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -4022,7 +4078,7 @@
       <c r="AC71" s="3"/>
       <c r="AD71" s="53"/>
     </row>
-    <row r="72" spans="1:30" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:30" s="2" customFormat="1" ht="24">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -4057,7 +4113,7 @@
       <c r="AC72" s="3"/>
       <c r="AD72" s="53"/>
     </row>
-    <row r="73" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:30" s="2" customFormat="1">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -4103,7 +4159,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="74" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:30" s="2" customFormat="1">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -4140,7 +4196,7 @@
       <c r="AC74" s="3"/>
       <c r="AD74" s="53"/>
     </row>
-    <row r="75" spans="1:30" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:30" s="2" customFormat="1" ht="24">
       <c r="A75" s="4"/>
       <c r="B75" s="3" t="s">
         <v>58</v>
@@ -4182,7 +4238,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="76" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:30" s="2" customFormat="1">
       <c r="A76" s="4"/>
       <c r="C76" s="4" t="s">
         <v>59</v>
@@ -4214,7 +4270,7 @@
       <c r="AC76" s="3"/>
       <c r="AD76" s="53"/>
     </row>
-    <row r="77" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:30" s="2" customFormat="1">
       <c r="A77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="6" t="s">
@@ -4248,7 +4304,7 @@
       <c r="AC77" s="3"/>
       <c r="AD77" s="53"/>
     </row>
-    <row r="78" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:30" s="2" customFormat="1">
       <c r="A78" s="4"/>
       <c r="C78" s="4"/>
       <c r="E78" s="6" t="s">
@@ -4283,8 +4339,8 @@
       </c>
       <c r="Z78" s="3"/>
       <c r="AA78" s="3"/>
-      <c r="AB78" s="3" t="s">
-        <v>172</v>
+      <c r="AB78" s="77" t="s">
+        <v>182</v>
       </c>
       <c r="AC78" s="3" t="s">
         <v>1</v>
@@ -4293,7 +4349,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:30" s="2" customFormat="1">
       <c r="A79" s="4"/>
       <c r="C79" s="4"/>
       <c r="E79" s="6" t="s">
@@ -4328,7 +4384,7 @@
       <c r="AC79" s="3"/>
       <c r="AD79" s="53"/>
     </row>
-    <row r="80" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:30" s="2" customFormat="1">
       <c r="A80" s="4"/>
       <c r="C80" s="4"/>
       <c r="E80" s="6" t="s">
@@ -4358,7 +4414,7 @@
       <c r="AC80" s="3"/>
       <c r="AD80" s="53"/>
     </row>
-    <row r="81" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:30" s="2" customFormat="1">
       <c r="A81" s="4"/>
       <c r="C81" s="4"/>
       <c r="E81" s="6"/>
@@ -4393,7 +4449,7 @@
       <c r="AC81" s="3"/>
       <c r="AD81" s="53"/>
     </row>
-    <row r="82" spans="1:30" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:30" s="2" customFormat="1" ht="24">
       <c r="A82" s="4"/>
       <c r="B82" s="3" t="s">
         <v>62</v>
@@ -4426,7 +4482,7 @@
       <c r="AC82" s="3"/>
       <c r="AD82" s="53"/>
     </row>
-    <row r="83" spans="1:30" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:30" s="2" customFormat="1">
       <c r="A83" s="4"/>
       <c r="C83" s="6" t="s">
         <v>63</v>
@@ -4463,7 +4519,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="84" spans="1:30" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:30" s="2" customFormat="1" ht="24">
       <c r="A84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="6" t="s">
@@ -4506,7 +4562,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="85" spans="1:30" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:30" s="2" customFormat="1" ht="24">
       <c r="A85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
@@ -4542,7 +4598,7 @@
       <c r="AC85" s="3"/>
       <c r="AD85" s="53"/>
     </row>
-    <row r="86" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:30" s="2" customFormat="1">
       <c r="A86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
@@ -4576,7 +4632,7 @@
       <c r="AC86" s="3"/>
       <c r="AD86" s="53"/>
     </row>
-    <row r="87" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:30" s="2" customFormat="1">
       <c r="A87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" t="s">
@@ -4619,7 +4675,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:30" s="2" customFormat="1">
       <c r="A88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
@@ -4655,7 +4711,7 @@
       <c r="AC88" s="3"/>
       <c r="AD88" s="53"/>
     </row>
-    <row r="89" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:30" s="2" customFormat="1">
       <c r="A89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
@@ -4682,7 +4738,7 @@
       <c r="AC89" s="3"/>
       <c r="AD89" s="53"/>
     </row>
-    <row r="90" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:30" s="2" customFormat="1">
       <c r="A90" s="4"/>
       <c r="C90" s="4"/>
       <c r="E90" s="6"/>
@@ -4708,7 +4764,7 @@
       <c r="AC90" s="3"/>
       <c r="AD90" s="53"/>
     </row>
-    <row r="91" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:30" s="2" customFormat="1">
       <c r="B91" s="20" t="s">
         <v>6</v>
       </c>
@@ -4738,7 +4794,7 @@
       <c r="AC91" s="3"/>
       <c r="AD91" s="53"/>
     </row>
-    <row r="92" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:30" s="2" customFormat="1">
       <c r="B92" s="20" t="s">
         <v>22</v>
       </c>
@@ -4770,7 +4826,7 @@
       <c r="AC92" s="3"/>
       <c r="AD92" s="53"/>
     </row>
-    <row r="93" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:30" s="2" customFormat="1">
       <c r="B93" s="20" t="s">
         <v>6</v>
       </c>
@@ -4800,7 +4856,7 @@
       <c r="AC93" s="3"/>
       <c r="AD93" s="53"/>
     </row>
-    <row r="94" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:30" s="2" customFormat="1">
       <c r="A94" s="4"/>
       <c r="B94" s="4" t="s">
         <v>23</v>
@@ -4833,7 +4889,7 @@
       <c r="AC94" s="3"/>
       <c r="AD94" s="53"/>
     </row>
-    <row r="95" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:30" s="4" customFormat="1">
       <c r="C95" s="4" t="s">
         <v>24</v>
       </c>
@@ -4848,7 +4904,7 @@
       <c r="AC95" s="6"/>
       <c r="AD95" s="73"/>
     </row>
-    <row r="96" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:30" s="2" customFormat="1">
       <c r="B96" s="20" t="s">
         <v>6</v>
       </c>
@@ -4876,7 +4932,7 @@
       <c r="AC96" s="3"/>
       <c r="AD96" s="53"/>
     </row>
-    <row r="97" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:30" s="2" customFormat="1">
       <c r="B97" s="20" t="s">
         <v>65</v>
       </c>
@@ -4904,7 +4960,7 @@
       <c r="AC97" s="3"/>
       <c r="AD97" s="53"/>
     </row>
-    <row r="98" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:30" s="2" customFormat="1">
       <c r="B98" s="20" t="s">
         <v>6</v>
       </c>
@@ -4932,7 +4988,7 @@
       <c r="AC98" s="3"/>
       <c r="AD98" s="53"/>
     </row>
-    <row r="99" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:30" s="2" customFormat="1">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -4974,7 +5030,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="100" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:30" s="2" customFormat="1">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -5007,7 +5063,7 @@
       <c r="AC100" s="3"/>
       <c r="AD100" s="53"/>
     </row>
-    <row r="101" spans="1:30" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:30" s="2" customFormat="1" ht="48">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -5052,7 +5108,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="102" spans="1:30" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:30" s="2" customFormat="1" ht="60">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -5089,7 +5145,7 @@
       <c r="AC102" s="3"/>
       <c r="AD102" s="53"/>
     </row>
-    <row r="103" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:30" s="2" customFormat="1">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -5126,7 +5182,7 @@
       <c r="AC103" s="3"/>
       <c r="AD103" s="53"/>
     </row>
-    <row r="104" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:30" s="2" customFormat="1">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -5173,7 +5229,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="105" spans="1:30" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:30" s="2" customFormat="1" ht="60">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -5220,7 +5276,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="106" spans="1:30" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:30" s="2" customFormat="1" ht="24">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -5255,7 +5311,7 @@
       <c r="AC106" s="3"/>
       <c r="AD106" s="53"/>
     </row>
-    <row r="107" spans="1:30" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:30" s="2" customFormat="1" ht="36">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -5292,7 +5348,7 @@
       <c r="AC107" s="3"/>
       <c r="AD107" s="53"/>
     </row>
-    <row r="108" spans="1:30" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:30" s="2" customFormat="1" ht="36">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -5334,7 +5390,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="109" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:30" s="2" customFormat="1">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -5367,7 +5423,7 @@
       <c r="AC109" s="3"/>
       <c r="AD109" s="53"/>
     </row>
-    <row r="110" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:30" s="2" customFormat="1">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -5402,7 +5458,7 @@
       <c r="AC110" s="3"/>
       <c r="AD110" s="53"/>
     </row>
-    <row r="111" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:30" s="2" customFormat="1">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -5437,7 +5493,7 @@
       <c r="AC111" s="3"/>
       <c r="AD111" s="53"/>
     </row>
-    <row r="112" spans="1:30" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:30" s="2" customFormat="1">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -5484,7 +5540,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="113" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:30" s="2" customFormat="1">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -5528,7 +5584,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="114" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:30" s="2" customFormat="1">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -5563,7 +5619,7 @@
       <c r="AC114" s="3"/>
       <c r="AD114" s="53"/>
     </row>
-    <row r="115" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:30" s="2" customFormat="1">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -5602,7 +5658,7 @@
       <c r="AC115" s="3"/>
       <c r="AD115" s="53"/>
     </row>
-    <row r="116" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:30" s="2" customFormat="1">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
@@ -5639,7 +5695,7 @@
       <c r="AC116" s="3"/>
       <c r="AD116" s="53"/>
     </row>
-    <row r="117" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:30" s="2" customFormat="1">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
@@ -5676,7 +5732,7 @@
       <c r="AC117" s="3"/>
       <c r="AD117" s="53"/>
     </row>
-    <row r="118" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:30" s="2" customFormat="1">
       <c r="A118" s="4"/>
       <c r="B118" s="4" t="s">
         <v>6</v>
@@ -5707,7 +5763,7 @@
       <c r="AC118" s="3"/>
       <c r="AD118" s="53"/>
     </row>
-    <row r="119" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:30" s="2" customFormat="1">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
@@ -5736,7 +5792,7 @@
       <c r="AC119" s="3"/>
       <c r="AD119" s="53"/>
     </row>
-    <row r="120" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:30" s="2" customFormat="1">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
@@ -5765,7 +5821,7 @@
       <c r="AC120" s="3"/>
       <c r="AD120" s="53"/>
     </row>
-    <row r="121" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:30" s="2" customFormat="1">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
@@ -5794,7 +5850,7 @@
       <c r="AC121" s="3"/>
       <c r="AD121" s="53"/>
     </row>
-    <row r="122" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:30" s="2" customFormat="1">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -5821,7 +5877,7 @@
       <c r="AC122" s="3"/>
       <c r="AD122" s="53"/>
     </row>
-    <row r="123" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:30" s="2" customFormat="1">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -5848,7 +5904,7 @@
       <c r="AC123" s="3"/>
       <c r="AD123" s="53"/>
     </row>
-    <row r="124" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:30" s="2" customFormat="1">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -5875,7 +5931,7 @@
       <c r="AC124" s="3"/>
       <c r="AD124" s="53"/>
     </row>
-    <row r="125" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:30" s="2" customFormat="1">
       <c r="A125" s="4"/>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
@@ -5899,7 +5955,7 @@
       <c r="AC125" s="3"/>
       <c r="AD125" s="53"/>
     </row>
-    <row r="126" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:30" s="2" customFormat="1">
       <c r="A126" s="4"/>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
@@ -5922,7 +5978,7 @@
       <c r="AC126" s="3"/>
       <c r="AD126" s="53"/>
     </row>
-    <row r="127" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:30" s="2" customFormat="1">
       <c r="A127" s="4"/>
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
@@ -5946,7 +6002,7 @@
       <c r="AC127" s="3"/>
       <c r="AD127" s="53"/>
     </row>
-    <row r="128" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:30" s="2" customFormat="1">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -5971,7 +6027,7 @@
       <c r="AC128" s="3"/>
       <c r="AD128" s="53"/>
     </row>
-    <row r="129" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:30" s="2" customFormat="1">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -5996,7 +6052,7 @@
       <c r="AC129" s="3"/>
       <c r="AD129" s="53"/>
     </row>
-    <row r="130" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:30" s="2" customFormat="1">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -6020,7 +6076,7 @@
       <c r="AC130" s="3"/>
       <c r="AD130" s="53"/>
     </row>
-    <row r="131" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:30" s="2" customFormat="1">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -6044,7 +6100,7 @@
       <c r="AC131" s="3"/>
       <c r="AD131" s="53"/>
     </row>
-    <row r="132" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:30" s="2" customFormat="1">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -6069,7 +6125,7 @@
       <c r="AC132" s="3"/>
       <c r="AD132" s="53"/>
     </row>
-    <row r="133" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:30" s="2" customFormat="1">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -6096,7 +6152,7 @@
       <c r="AC133" s="3"/>
       <c r="AD133" s="53"/>
     </row>
-    <row r="134" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:30" s="2" customFormat="1">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -6125,7 +6181,7 @@
       <c r="AC134" s="3"/>
       <c r="AD134" s="53"/>
     </row>
-    <row r="135" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:30" s="2" customFormat="1">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -6154,7 +6210,7 @@
       <c r="AC135" s="3"/>
       <c r="AD135" s="53"/>
     </row>
-    <row r="136" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:30" s="2" customFormat="1">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
@@ -6183,7 +6239,7 @@
       <c r="AC136" s="3"/>
       <c r="AD136" s="53"/>
     </row>
-    <row r="137" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:30" s="2" customFormat="1">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
@@ -6212,7 +6268,7 @@
       <c r="AC137" s="3"/>
       <c r="AD137" s="53"/>
     </row>
-    <row r="138" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:30" s="2" customFormat="1">
       <c r="A138" s="4"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
@@ -6239,7 +6295,7 @@
       <c r="AC138" s="3"/>
       <c r="AD138" s="53"/>
     </row>
-    <row r="139" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:30" s="2" customFormat="1">
       <c r="A139" s="4"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
@@ -6266,7 +6322,7 @@
       <c r="AC139" s="3"/>
       <c r="AD139" s="53"/>
     </row>
-    <row r="140" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:30" s="2" customFormat="1">
       <c r="A140" s="4"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
@@ -6293,7 +6349,7 @@
       <c r="AC140" s="3"/>
       <c r="AD140" s="53"/>
     </row>
-    <row r="141" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:30" s="2" customFormat="1">
       <c r="A141" s="4"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
@@ -6320,7 +6376,7 @@
       <c r="AC141" s="3"/>
       <c r="AD141" s="53"/>
     </row>
-    <row r="142" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:30" s="2" customFormat="1">
       <c r="A142" s="4"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
@@ -6347,7 +6403,7 @@
       <c r="AC142" s="3"/>
       <c r="AD142" s="53"/>
     </row>
-    <row r="143" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:30" s="2" customFormat="1">
       <c r="A143" s="4"/>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
@@ -6374,7 +6430,7 @@
       <c r="AC143" s="3"/>
       <c r="AD143" s="53"/>
     </row>
-    <row r="144" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:30" s="2" customFormat="1">
       <c r="A144" s="4"/>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
@@ -6401,7 +6457,7 @@
       <c r="AC144" s="3"/>
       <c r="AD144" s="53"/>
     </row>
-    <row r="145" spans="1:30" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:30" s="2" customFormat="1" ht="26.25" customHeight="1">
       <c r="A145" s="4"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
@@ -6428,7 +6484,7 @@
       <c r="AC145" s="3"/>
       <c r="AD145" s="53"/>
     </row>
-    <row r="146" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:30" s="2" customFormat="1">
       <c r="A146" s="4"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
@@ -6454,7 +6510,7 @@
       <c r="AC146" s="3"/>
       <c r="AD146" s="53"/>
     </row>
-    <row r="147" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:30" s="2" customFormat="1">
       <c r="A147" s="4"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
@@ -6479,7 +6535,7 @@
       <c r="AC147" s="3"/>
       <c r="AD147" s="53"/>
     </row>
-    <row r="148" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:30" s="2" customFormat="1">
       <c r="A148" s="4"/>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
@@ -6506,7 +6562,7 @@
       <c r="AC148" s="3"/>
       <c r="AD148" s="53"/>
     </row>
-    <row r="149" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:30" s="2" customFormat="1">
       <c r="A149" s="4"/>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
@@ -6534,7 +6590,7 @@
       <c r="AC149" s="3"/>
       <c r="AD149" s="53"/>
     </row>
-    <row r="150" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:30" s="2" customFormat="1">
       <c r="I150" s="3"/>
       <c r="U150" s="10"/>
       <c r="V150" s="42"/>
@@ -6544,7 +6600,7 @@
       <c r="AC150" s="3"/>
       <c r="AD150" s="53"/>
     </row>
-    <row r="151" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:30" s="2" customFormat="1">
       <c r="J151" s="3"/>
       <c r="U151" s="10"/>
       <c r="V151" s="42"/>
@@ -6554,7 +6610,7 @@
       <c r="AC151" s="3"/>
       <c r="AD151" s="53"/>
     </row>
-    <row r="152" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:30" s="2" customFormat="1">
       <c r="U152" s="10"/>
       <c r="V152" s="42"/>
       <c r="W152" s="42"/>
@@ -6563,7 +6619,7 @@
       <c r="AC152" s="3"/>
       <c r="AD152" s="53"/>
     </row>
-    <row r="153" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:30" s="2" customFormat="1">
       <c r="U153" s="10"/>
       <c r="V153" s="42"/>
       <c r="W153" s="42"/>
@@ -6572,7 +6628,7 @@
       <c r="AC153" s="3"/>
       <c r="AD153" s="53"/>
     </row>
-    <row r="154" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:30" s="2" customFormat="1">
       <c r="U154" s="10"/>
       <c r="V154" s="42"/>
       <c r="W154" s="42"/>
@@ -6581,7 +6637,7 @@
       <c r="AC154" s="3"/>
       <c r="AD154" s="53"/>
     </row>
-    <row r="155" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:30" s="2" customFormat="1">
       <c r="U155" s="10"/>
       <c r="V155" s="42"/>
       <c r="W155" s="42"/>
@@ -6590,7 +6646,7 @@
       <c r="AC155" s="3"/>
       <c r="AD155" s="53"/>
     </row>
-    <row r="156" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:30" s="2" customFormat="1">
       <c r="U156" s="10"/>
       <c r="V156" s="42"/>
       <c r="W156" s="42"/>
@@ -6599,7 +6655,7 @@
       <c r="AC156" s="3"/>
       <c r="AD156" s="53"/>
     </row>
-    <row r="157" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:30" s="2" customFormat="1">
       <c r="U157" s="10"/>
       <c r="V157" s="42"/>
       <c r="W157" s="42"/>
@@ -6608,7 +6664,7 @@
       <c r="AC157" s="3"/>
       <c r="AD157" s="53"/>
     </row>
-    <row r="158" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:30" s="2" customFormat="1">
       <c r="U158" s="10"/>
       <c r="V158" s="42"/>
       <c r="W158" s="42"/>
@@ -6617,7 +6673,7 @@
       <c r="AC158" s="3"/>
       <c r="AD158" s="53"/>
     </row>
-    <row r="159" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:30" s="2" customFormat="1">
       <c r="U159" s="10"/>
       <c r="V159" s="42"/>
       <c r="W159" s="42"/>
@@ -6626,7 +6682,7 @@
       <c r="AC159" s="3"/>
       <c r="AD159" s="53"/>
     </row>
-    <row r="160" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:30" s="2" customFormat="1">
       <c r="U160" s="10"/>
       <c r="V160" s="42"/>
       <c r="W160" s="42"/>
@@ -6635,7 +6691,7 @@
       <c r="AC160" s="3"/>
       <c r="AD160" s="53"/>
     </row>
-    <row r="161" spans="21:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="21:30" s="2" customFormat="1">
       <c r="U161" s="10"/>
       <c r="V161" s="42"/>
       <c r="W161" s="42"/>
@@ -6644,7 +6700,7 @@
       <c r="AC161" s="3"/>
       <c r="AD161" s="53"/>
     </row>
-    <row r="162" spans="21:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="21:30" s="2" customFormat="1">
       <c r="U162" s="10"/>
       <c r="V162" s="42"/>
       <c r="W162" s="42"/>
@@ -6653,7 +6709,7 @@
       <c r="AC162" s="3"/>
       <c r="AD162" s="53"/>
     </row>
-    <row r="163" spans="21:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="21:30" s="2" customFormat="1">
       <c r="U163" s="10"/>
       <c r="V163" s="42"/>
       <c r="W163" s="42"/>
@@ -6662,7 +6718,7 @@
       <c r="AC163" s="3"/>
       <c r="AD163" s="53"/>
     </row>
-    <row r="164" spans="21:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="21:30" s="2" customFormat="1">
       <c r="U164" s="10"/>
       <c r="V164" s="42"/>
       <c r="W164" s="42"/>
@@ -6671,7 +6727,7 @@
       <c r="AC164" s="3"/>
       <c r="AD164" s="53"/>
     </row>
-    <row r="165" spans="21:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="21:30" s="2" customFormat="1">
       <c r="U165" s="10"/>
       <c r="V165" s="42"/>
       <c r="W165" s="42"/>
@@ -6680,7 +6736,7 @@
       <c r="AC165" s="3"/>
       <c r="AD165" s="53"/>
     </row>
-    <row r="166" spans="21:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="21:30" s="2" customFormat="1">
       <c r="U166" s="10"/>
       <c r="V166" s="42"/>
       <c r="W166" s="42"/>
@@ -6696,7 +6752,12 @@
     <mergeCell ref="V3:W3"/>
   </mergeCells>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="8" scale="80" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="80" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>